<commit_message>
precio partido en moneda y valor
</commit_message>
<xml_diff>
--- a/app/database/Parametros.xlsx
+++ b/app/database/Parametros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2026\Gesglos\booking_scraper\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39684F42-15D1-4A64-AC05-679E74D060C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DA4F0A-CEF1-4327-A2A0-05E52475B63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21336" windowHeight="11376" xr2:uid="{9E98B23C-6360-4275-ADF1-08EC9DEFEBC7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="41">
   <si>
     <t>Hotel</t>
   </si>
@@ -158,6 +158,12 @@
   <si>
     <t>Hotel Campestre Alto lindo en Guatapé</t>
   </si>
+  <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>Botánica Casa Hotel Manila by HOUSY</t>
+  </si>
 </sst>
 </file>
 
@@ -258,7 +264,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +392,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -471,6 +483,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -997,11 +1012,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490BB3E7-AA76-410D-8D51-AC55157784CD}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,6 +1060,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
     </row>
@@ -1061,6 +1085,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FCB63C-18F2-44BE-92D8-19338A9887F9}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1591,6 +1616,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4176F2-6A77-4C34-8EDA-976C834D1280}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:J776"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">

</xml_diff>